<commit_message>
adding in data after the election for tds
</commit_message>
<xml_diff>
--- a/data/tds-topics-election.xlsx
+++ b/data/tds-topics-election.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annafetter/Documents/political-satire/r-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3676B200-1649-2742-9155-436D3539EC6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83C3C71-DBE7-DE45-8958-6A2CCF319DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="311">
   <si>
     <t>date</t>
   </si>
@@ -120,6 +120,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -274,6 +275,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -376,6 +378,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -467,6 +470,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -542,6 +546,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -589,6 +594,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -673,6 +679,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -705,6 +712,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -765,6 +773,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -832,6 +841,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -871,6 +881,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -934,6 +945,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -976,6 +988,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -1032,6 +1045,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -1066,6 +1080,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -1096,6 +1111,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -1126,6 +1142,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -1176,6 +1193,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -1200,6 +1218,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -1245,6 +1264,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -1303,6 +1323,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -1343,6 +1364,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -1391,6 +1413,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -1427,6 +1450,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -1464,6 +1488,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -1562,6 +1587,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -1595,6 +1621,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -1649,6 +1676,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -1685,6 +1713,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -1697,6 +1726,539 @@
 Positioned as a defining political message |
 | Kamala Harris | No Specific Mentions | No immigration policy discussion |
 | Broader Context | Political Narrative | Immigration used as a lens to discuss political messaging |</t>
+  </si>
+  <si>
+    <t>Jon Stewart and The Best F**king News Team Take on Election Night 2024 | The Daily Show</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://www.youtube.com/watch?v=ZjMAfRq7V_s&amp;list=PLLUTEX3bD4_rdg94fNT3jT6S8lENEztyf&amp;index=48</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Lt. Gov. Garlin Gilchrist II - Staying Optimistic for the Future on Election Night | The Daily Show </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://www.youtube.com/watch?v=wmkF9yBnUbI&amp;list=PLLUTEX3bD4_rdg94fNT3jT6S8lENEztyf&amp;index=49</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Positive Policy Approach
+Credited with supporting reproductive freedom
+Associated with Michigan's constitutional amendment protecting reproductive rights
+Positioned as a champion of women's reproductive rights
+Framed as part of a broader movement for reproductive justice</t>
+  </si>
+  <si>
+    <t>Inflammatory Immigration Rhetoric
+Called for "ban on all Muslims traveling to America"
+Controversial statements about immigrant communities
+Specifically mentioned in context of Dearborn's Arab-American community
+Portrayed as divisive and discriminatory
+No substantive immigration policy proposals discussed</t>
+  </si>
+  <si>
+    <t>Optimistic Economic Vision
+Associated with belief in technological innovation
+Positioned as supporting manufacturing and future economic growth
+Framed as an advocate for:
+Electric vehicle industry
+Clean energy development
+Technological advancement
+Presented as having faith in Michigan's economic potential
+Emphasized hope and future-oriented economic thinking</t>
+  </si>
+  <si>
+    <t>Pessimistic Economic Narrative
+Claimed Michigan "can't win the electric vehicle race"
+Suggested China would beat America economically
+Portrayed as defeatist about manufacturing and technology
+Criticized for lack of belief in American industrial potential
+No concrete economic development proposals mentioned</t>
+  </si>
+  <si>
+    <t>Gov. Katie Hobbs – Arizona as an Election Swing State &amp; Enshrining Abortion Rights | The Daily Show</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=_jK1FvuaBpA&amp;list=PLLUTEX3bD4_rdg94fNT3jT6S8lENEztyf&amp;index=50 </t>
+  </si>
+  <si>
+    <t>Desi Lydic Reacts to Trump's Election Win &amp; the Media's Blame Game | The Daily Show</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=hPHH5trgC1w&amp;list=PLLUTEX3bD4_rdg94fNT3jT6S8lENEztyf&amp;index=51 </t>
+  </si>
+  <si>
+    <t>Accused of being "too far left"
+Criticized for lack of clear positioning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accused of not being pro-Israel enough
+Simultaneously criticized for not being pro-Palestinian enough
+No specific immigration policy details provided </t>
+  </si>
+  <si>
+    <t>Demographic Victory | Immigration-Adjacent Discussion:
+Noted for winning diverse demographic groups
+Mentioned as breaking through Midwest "blue wall"</t>
+  </si>
+  <si>
+    <t>Accused of not embracing centrists
+Criticized for association with Joe Biden
+No substantive economic policy discussion</t>
+  </si>
+  <si>
+    <t>Demographic Economic Narrative | Victory Interpreted Through Economic Lens:
+Portrayed as winning across various voter demographics
+No specific economic policy proposals mentioned
+Economic success implied through electoral victory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tressie McMillan Cottom - Identity Politics and the 2024 Election | The Daily Show </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://www.youtube.com/watch?v=nno64FGj8d0&amp;list=PLLUTEX3bD4_rdg94fNT3jT6S8lENEztyf&amp;index=52</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Briefly mentioned in context of young women's fears
+Noted that some women might not believe a female president would help</t>
+  </si>
+  <si>
+    <t>Voters noted ability to "parse the difference between defending abortion but voting for Trump"</t>
+  </si>
+  <si>
+    <t>Discussed as part of simple campaign narrative
+Quoted as saying "oh, the border, I'll fix it"
+No detailed policy proposals
+Presented as part of Trump's ability to tell a compelling story</t>
+  </si>
+  <si>
+    <t>Focuses on making people "feel like they're winning"
+Promises without specific plans
+Addresses economic anxieties through emotional storytelling:
+"Things are bad. I will make it good."
+Targets fundamental economic concerns:
+Housing expenses
+Child care costs
+Caring for parents
+Provides a sense of certainty without concrete policy details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-Voters Teach Grace Kuhlenschmidt How to Not Give a F**k About Politics | The Daily Show </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=SqZTRREqzVM&amp;list=PLLUTEX3bD4_rdg94fNT3jT6S8lENEztyf&amp;index=53 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biden &amp; Harris Vow Peaceful Transition &amp; Trump’s Potential Cabinet Is a Motley Crew | The Daily Show </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://www.youtube.com/watch?v=aO1C5A0ZCRo&amp;list=PLLUTEX3bD4_rdg94fNT3jT6S8lENEztyf&amp;index=54</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Implied racist approach to immigration through comedic voice actor line: "I lied a lot, and I was super racist" (8:01-8:02)</t>
+  </si>
+  <si>
+    <t>Superficial Economic Mention | Economic challenges reduced to:
+Egg prices
+Vague references to legislation
+No substantive economic policy analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emily Ngo - Unpacking Election as a Political Journalist &amp; Jury Duty with Trump | The Daily Show </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://www.youtube.com/watch?v=DOkWM97KItY&amp;list=PLLUTEX3bD4_rdg94fNT3jT6S8lENEztyf&amp;index=55</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Made gains with Latino voters in the Bronx (14:12-14:14)
+Discussed voter perceptions about border security (4:10-4:17)
+Voters concerned about "migrants and people who arrive here and stay illegally"</t>
+  </si>
+  <si>
+    <t>Discussed as appealing to voters concerned about inflation (4:10)
+Portrayed as understanding economic anxieties of voters
+Highlighted gains in working-class American support (2:31-2:38)
+Mentioned making electoral gains in economically challenged areas (3:14-3:20)</t>
+  </si>
+  <si>
+    <t>Jon Stewart &amp; The News Team Cover The Fallout From the 2024 Election | The Daily Show</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://www.youtube.com/watch?v=TNVARon2rvE&amp;list=PLLUTEX3bD4_rdg94fNT3jT6S8lENEztyf&amp;index=57</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Brief mention of potential voter concerns
+Criticized for not addressing reproductive rights effectively</t>
+  </si>
+  <si>
+    <t>Made gains with Latino voters
+Discussed border security concerns
+Highlighted support from diverse demographic groups
+Implied tough stance on immigration</t>
+  </si>
+  <si>
+    <t>Portrayed as understanding voter economic anxieties
+Discussed making gains with working-class Americans
+Implied economic appeal across demographics</t>
+  </si>
+  <si>
+    <t>Jon Stewart On What Went Wrong For Democrats | The Daily Show</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://www.youtube.com/watch?v=TKBJoj4XyFc&amp;list=PLLUTEX3bD4_rdg94fNT3jT6S8lENEztyf&amp;index=58</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Criticized for "wildly overestimating the power of the abortion issue" (7:23)
+No substantive policy discussion</t>
+  </si>
+  <si>
+    <t>Democrats portrayed as tough on immigration
+Campaign ads focusing on border security (10:41-10:49)
+Rhetoric about "border crisis" and "migrant crisis"</t>
+  </si>
+  <si>
+    <t>Criticized for spending "too little time talking about the economy" (7:19)
+No specific economic policy proposals discussed</t>
+  </si>
+  <si>
+    <t>Implied Economic Narrative | Voter Perception:
+Democrats portrayed as disconnected from economic concerns
+Narrative that government "wasn't working for them" (13:32-13:41)
+Suggestion that Democrats were "taking their hard-earned money" (13:37-13:41)</t>
+  </si>
+  <si>
+    <t>Trump Adds Noem, Rubio, Stefanik to Cabinet, With Elon on Watch | The Daily Show</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://www.youtube.com/watch?v=p6b9PSkopnw&amp;list=PLLUTEX3bD4_rdg94fNT3jT6S8lENEztyf&amp;index=58</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Implied mass deportation plans (0:25-0:33)
+Potential border control focus through appointees
+Kristi Noem's potential Homeland Security role tied to border control (1:13-1:15)</t>
+  </si>
+  <si>
+    <t>Mention of bringing "back American jobs to the auto industry" (2:49-2:53)
+Discussion of "energy dominance" (2:44-2:49)
+Proposal to roll back business regulations (2:56-3:02)</t>
+  </si>
+  <si>
+    <t>Trump Acts Cordial With Biden While Gaetz, Gabbard, and Hegseth Score Nominations | The Daily Show</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://www.youtube.com/watch?v=klEF0fjTOsE&amp;list=PLLUTEX3bD4_rdg94fNT3jT6S8lENEztyf&amp;index=60</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Pete Hegseth's comments on women in military roles
+Suggestion that women should "get pregnant" instead of serving in combat (7:11-7:14)
+Implied restrictive stance on women's roles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potential mass deportation plans implied by cabinet picks
+Kristi Noem's potential Homeland Security role suggests strict border control approach
+No specific detailed immigration policy proposals </t>
+  </si>
+  <si>
+    <t>Implied deregulation through cabinet appointments
+Pete Hegseth's commentary on "protecting businesses"
+Emphasis on "American jobs" and "energy dominance"
+No comprehensive economic policy detailed</t>
+  </si>
+  <si>
+    <t>Dulcé Sloan Makes a Time Capsule of American Art &amp; Culture Before Trump Bans It All | The Daily Show</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://www.youtube.com/watch?v=Jjdfm-UqKy4&amp;list=PLLUTEX3bD4_rdg94fNT3jT6S8lENEztyf&amp;index=60</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Indirect reference to immigration through commentary on previous presidency
+Mentioned in context of societal breakdown (0:05-0:16)
+No specific immigration policy proposals</t>
+  </si>
+  <si>
+    <t>Trump Nominates RFK Jr. and Matt Gaetz In Latest Shock Moves | The Daily Show</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=3FaWC6LMniU&amp;list=PLLUTEX3bD4_rdg94fNT3jT6S8lENEztyf&amp;index=61 </t>
+  </si>
+  <si>
+    <t>Appointment of Robert F. Kennedy Jr. as Secretary of Health and Human Services
+Implies potentially controversial approach to public health
+Satirical reference to "Unpasteurized whale juice" (0:19)
+Suggestion of anti-vaccination stance through RFK Jr. appointment</t>
+  </si>
+  <si>
+    <t>Charlamagne Tha God Issues a Plea to Trump: “Leave the Constitution in One Piece” | The Daily Show</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=08ZE2p0TQng&amp;list=PLLUTEX3bD4_rdg94fNT3jT6S8lENEztyf&amp;index=62 </t>
+  </si>
+  <si>
+    <t>Mentioned in context of potential authoritarian approach
+No specific immigration policy proposals
+Implied potential for aggressive governmental action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hypothetical suggestion of potential budget skimming (5:29-5:36)
+Joke about potentially destroying the economy (5:55-6:02)
+Described as "normal Republican president stuff" economically
+No detailed economic policy proposals </t>
+  </si>
+  <si>
+    <t>Jon Stewart's Post-Election Analysis &amp; Klepper on Trump's Cabinet Nominations | The Daily Show</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=RaWfrvQ8Zq0&amp;list=PLLUTEX3bD4_rdg94fNT3jT6S8lENEztyf&amp;index=63 </t>
+  </si>
+  <si>
+    <t>Mentioned as "wildly overestimating the power of the abortion issue" (5:35)</t>
+  </si>
+  <si>
+    <t>Controversial Reproductive Policy Implications | Indirect References:
+Pete Hegseth's comments on women in military roles (27:14-27:45)
+Suggested women should "get pregnant" to risk their lives
+Implied restrictive stance on women's roles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Campaign ads focusing on border security (8:53-9:04)
+Slogans like "We can't let China steal Wisconsin jobs" (9:50)
+"Benefits for illegal immigrants? No way" (9:50)
+Implied strict border control approach </t>
+  </si>
+  <si>
+    <t>Criticized for spending "too little time talking about the economy" (5:29)</t>
+  </si>
+  <si>
+    <t>Superficial Economic Commentary:
+Lee Zeldin's EPA pick discussing "energy dominance" (14:51-15:03)
+Promises to "bring back American jobs to the auto industry"
+Proposal to "roll back regulations" affecting businesses</t>
+  </si>
+  <si>
+    <t>Jon Stewart Urges Dems to Fight Like Republicans and Exploit Loopholes | The Daily Show</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>https://www.youtube.com/watch?v=HNcmo-K5Xsg&amp;list=PLLUTEX3bD4_rdg94fNT3jT6S8lENEztyf&amp;index=64</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Brief mention in Joe and Mika's Mar-a-Lago meeting discussion (11:15-11:19)
+Abortion mentioned as one of the "issues" discussed</t>
+  </si>
+  <si>
+    <t>Implied strict immigration stance
+Discussed in context of legislative constraints</t>
+  </si>
+  <si>
+    <t>Which Stocks Should You Buy During the Trump Administration? | The Daily Show</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=s0bJfUZj-ho&amp;list=PLLUTEX3bD4_rdg94fNT3jT6S8lENEztyf&amp;index=65 </t>
+  </si>
+  <si>
+    <t>Selection of Tom Homan as "border czar" (0:20-0:25)
+Significant impact on private prison stocks (0:20-0:37)
+Implied strict immigration enforcement approach
+Two private prison companies saw 56% stock increase</t>
+  </si>
+  <si>
+    <t>Impact on various stock markets
+Private prison stocks rising (0:20-0:37)
+Climate change policy affecting energy stocks (1:25-1:45)
+Dental supply stocks impacted by cabinet picks (2:42-3:01)
+Implied deregulation and business-friendly approach</t>
+  </si>
+  <si>
+    <t>Trump's TV Administration Adds Dr. Oz and Linda McMahon | The Daily Show</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=ZdddaTrQdrI&amp;list=PLLUTEX3bD4_rdg94fNT3jT6S8lENEztyf&amp;index=67 </t>
   </si>
 </sst>
 </file>
@@ -1705,9 +2267,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mmm\ d\,\ yyyy"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1774,6 +2336,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1795,7 +2364,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1827,15 +2396,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2054,10 +2626,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O53"/>
+  <dimension ref="A1:O67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4138,29 +4710,789 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="5:14" ht="13" x14ac:dyDescent="0.15">
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
-      <c r="M49" s="2"/>
+    <row r="49" spans="1:14" ht="112" x14ac:dyDescent="0.15">
+      <c r="A49" s="16">
+        <v>45602</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C49" s="18">
+        <v>1.337962962962963E-2</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K49" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L49" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M49" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="N49" s="2"/>
     </row>
-    <row r="53" spans="5:14" ht="13" x14ac:dyDescent="0.15">
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
-      <c r="M53" s="2"/>
+    <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="16">
+        <v>45603</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C50" s="18">
+        <v>5.5439814814814813E-3</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="K50" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L50" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M50" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="16">
+        <v>45604</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C51" s="18">
+        <v>3.9699074074074072E-3</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J51" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K51" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L51" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M51" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N51" s="5"/>
+    </row>
+    <row r="52" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="16">
+        <v>45605</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C52" s="18">
+        <v>0.01</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="J52" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="K52" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L52" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M52" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" ht="409.6" x14ac:dyDescent="0.15">
+      <c r="A53" s="16">
+        <v>45606</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C53" s="18">
+        <v>9.618055555555555E-3</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I53" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="K53" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L53" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M53" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="N53" s="2"/>
+    </row>
+    <row r="54" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="16">
+        <v>45607</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C54" s="18">
+        <v>2.3263888888888887E-3</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K54" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L54" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M54" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="16">
+        <v>45608</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C55" s="18">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J55" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="K55" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L55" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M55" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="16">
+        <v>45609</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C56" s="18">
+        <v>1.0115740740740741E-2</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="I56" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J56" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="K56" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L56" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M56" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="16">
+        <v>45610</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C57" s="18">
+        <v>1.5578703703703704E-2</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="I57" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J57" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="K57" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L57" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M57" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A58" s="16">
+        <v>45611</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C58" s="18">
+        <v>1.0231481481481482E-2</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="I58" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="J58" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="K58" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L58" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M58" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="16">
+        <v>45612</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="C59" s="18">
+        <v>7.4421296296296293E-3</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="I59" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J59" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="K59" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L59" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M59" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A60" s="16">
+        <v>45613</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C60" s="18">
+        <v>8.3101851851851843E-3</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="I60" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J60" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="K60" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L60" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M60" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A61" s="16">
+        <v>45614</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C61" s="18">
+        <v>2.476851851851852E-3</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="I61" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J61" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K61" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L61" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M61" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A62" s="16">
+        <v>45615</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C62" s="18">
+        <v>6.9097222222222225E-3</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I62" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J62" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K62" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L62" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M62" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N62" s="2"/>
+    </row>
+    <row r="63" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="16">
+        <v>45616</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C63" s="18">
+        <v>4.5949074074074078E-3</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J63" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="K63" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L63" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M63" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A64" s="16">
+        <v>45617</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C64" s="18">
+        <v>2.4583333333333332E-2</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="I64" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="J64" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="K64" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L64" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M64" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A65" s="16">
+        <v>45618</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C65" s="18">
+        <v>1.3587962962962963E-2</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="I65" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J65" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K65" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L65" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M65" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N65" s="2"/>
+    </row>
+    <row r="66" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A66" s="16">
+        <v>45619</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="C66" s="18">
+        <v>3.3449074074074076E-3</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H66" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="I66" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J66" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="K66" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L66" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M66" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A67" s="16">
+        <v>45620</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="C67" s="18">
+        <v>6.4699074074074077E-3</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I67" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J67" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K67" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L67" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M67" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4211,6 +5543,25 @@
     <hyperlink ref="D46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
     <hyperlink ref="D47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
     <hyperlink ref="D48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="D49" r:id="rId48" xr:uid="{B729D878-D1AD-9A4A-AD40-9438F269FEF2}"/>
+    <hyperlink ref="D50" r:id="rId49" xr:uid="{43B59424-3D98-5B4E-8EA2-13E251E8AE5E}"/>
+    <hyperlink ref="D51" r:id="rId50" xr:uid="{8D71A62C-7DE1-FD4E-B3DC-D54203C1E97D}"/>
+    <hyperlink ref="D52" r:id="rId51" xr:uid="{A54B9CFC-AB3B-BE4C-B084-591972F7A953}"/>
+    <hyperlink ref="D53" r:id="rId52" xr:uid="{5043F172-4FCB-0E4F-A926-E30BE5856A70}"/>
+    <hyperlink ref="D54" r:id="rId53" xr:uid="{4CE249C9-ABDF-2146-892E-62921ED279BE}"/>
+    <hyperlink ref="D55" r:id="rId54" xr:uid="{D47F9119-4674-194D-BD79-72BD866F31A3}"/>
+    <hyperlink ref="D56" r:id="rId55" xr:uid="{6AE75461-8ACC-654E-BB3E-D6903D094DB0}"/>
+    <hyperlink ref="D57" r:id="rId56" xr:uid="{31C01639-B790-894C-9258-40D6E3A91C4F}"/>
+    <hyperlink ref="D58" r:id="rId57" xr:uid="{D181C72E-7E31-CD40-B7BC-C6AB5416EA8D}"/>
+    <hyperlink ref="D59" r:id="rId58" xr:uid="{9C5967D6-7CE2-1B47-B355-C19B41A5B91E}"/>
+    <hyperlink ref="D60" r:id="rId59" xr:uid="{9C138342-5049-7C4E-BD14-7C20D49BF025}"/>
+    <hyperlink ref="D61" r:id="rId60" xr:uid="{AE3D96E0-B8BC-724D-9A54-89FA073153ED}"/>
+    <hyperlink ref="D62" r:id="rId61" xr:uid="{11830D5D-FD85-674B-BE0F-1EE53973BF80}"/>
+    <hyperlink ref="D63" r:id="rId62" xr:uid="{D2DF3EB6-D321-404F-8470-1BFD3E288301}"/>
+    <hyperlink ref="D64" r:id="rId63" xr:uid="{29C9207E-B5F8-E54C-AFF1-F7B28103D6FD}"/>
+    <hyperlink ref="D65" r:id="rId64" xr:uid="{788FB54E-863E-BC43-896B-9B6DA6160C83}"/>
+    <hyperlink ref="D66" r:id="rId65" xr:uid="{6344D27B-8AE1-BA45-8D72-0A44DCB0786C}"/>
+    <hyperlink ref="D67" r:id="rId66" xr:uid="{531DF8FA-7EC0-9B47-80CA-81BAC54D5E7D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>